<commit_message>
Updated full revin NN tuning to new laptop
</commit_message>
<xml_diff>
--- a/Metrics/newNNFullHyperTest.xlsx
+++ b/Metrics/newNNFullHyperTest.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -472,22 +472,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.08699999999999999</v>
+        <v>-0.078</v>
       </c>
       <c r="C2" t="n">
-        <v>1.699</v>
+        <v>1.693</v>
       </c>
       <c r="D2" t="n">
-        <v>7.502</v>
+        <v>7.44</v>
       </c>
       <c r="E2" t="n">
-        <v>2.739</v>
+        <v>2.728</v>
       </c>
       <c r="F2" t="n">
         <v>2.26</v>
       </c>
       <c r="G2" t="n">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3">
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.18</v>
+        <v>-0.042</v>
       </c>
       <c r="C3" t="n">
-        <v>1.759</v>
+        <v>1.67</v>
       </c>
       <c r="D3" t="n">
-        <v>0.749</v>
+        <v>0.662</v>
       </c>
       <c r="E3" t="n">
-        <v>0.865</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>0.609</v>
+        <v>0.57</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.168</v>
+        <v>-0.206</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.253</v>
+        <v>-0.034</v>
       </c>
       <c r="C4" t="n">
-        <v>1.806</v>
+        <v>1.665</v>
       </c>
       <c r="D4" t="n">
-        <v>0.219</v>
+        <v>0.18</v>
       </c>
       <c r="E4" t="n">
-        <v>0.468</v>
+        <v>0.424</v>
       </c>
       <c r="F4" t="n">
-        <v>0.376</v>
+        <v>0.32</v>
       </c>
       <c r="G4" t="n">
-        <v>0.028</v>
+        <v>-0.197</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.409</v>
+        <v>-0.509</v>
       </c>
       <c r="C5" t="n">
-        <v>1.906</v>
+        <v>1.97</v>
       </c>
       <c r="D5" t="n">
-        <v>1.107</v>
+        <v>1.186</v>
       </c>
       <c r="E5" t="n">
-        <v>1.052</v>
+        <v>1.089</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.846</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.204</v>
+        <v>-0.638</v>
       </c>
     </row>
     <row r="6">
@@ -572,22 +572,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.169</v>
+        <v>-0.04</v>
       </c>
       <c r="C6" t="n">
-        <v>1.534</v>
+        <v>1.669</v>
       </c>
       <c r="D6" t="n">
-        <v>0.737</v>
+        <v>0.922</v>
       </c>
       <c r="E6" t="n">
-        <v>0.858</v>
+        <v>0.96</v>
       </c>
       <c r="F6" t="n">
-        <v>0.899</v>
+        <v>0.841</v>
       </c>
       <c r="G6" t="n">
-        <v>0.59</v>
+        <v>-0.574</v>
       </c>
     </row>
     <row r="7">
@@ -597,22 +597,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.021</v>
+        <v>-0.012</v>
       </c>
       <c r="C7" t="n">
-        <v>1.656</v>
+        <v>1.651</v>
       </c>
       <c r="D7" t="n">
-        <v>1.28</v>
+        <v>1.267</v>
       </c>
       <c r="E7" t="n">
-        <v>1.131</v>
+        <v>1.126</v>
       </c>
       <c r="F7" t="n">
-        <v>1.003</v>
+        <v>0.992</v>
       </c>
       <c r="G7" t="n">
-        <v>0.219</v>
+        <v>-0.232</v>
       </c>
     </row>
     <row r="8">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.285</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>1.826</v>
+        <v>1.698</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44</v>
+        <v>0.372</v>
       </c>
       <c r="E8" t="n">
-        <v>0.663</v>
+        <v>0.61</v>
       </c>
       <c r="F8" t="n">
-        <v>0.572</v>
+        <v>0.483</v>
       </c>
       <c r="G8" t="n">
-        <v>0.389</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="9">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.371</v>
+        <v>-0.191</v>
       </c>
       <c r="C9" t="n">
-        <v>1.881</v>
+        <v>1.766</v>
       </c>
       <c r="D9" t="n">
-        <v>1.598</v>
+        <v>1.389</v>
       </c>
       <c r="E9" t="n">
-        <v>1.264</v>
+        <v>1.179</v>
       </c>
       <c r="F9" t="n">
-        <v>0.996</v>
+        <v>0.964</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.419</v>
+        <v>0.142</v>
       </c>
     </row>
     <row r="10">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.058</v>
+        <v>-0.005</v>
       </c>
       <c r="C10" t="n">
-        <v>1.606</v>
+        <v>1.646</v>
       </c>
       <c r="D10" t="n">
-        <v>0.844</v>
+        <v>0.901</v>
       </c>
       <c r="E10" t="n">
-        <v>0.919</v>
+        <v>0.949</v>
       </c>
       <c r="F10" t="n">
-        <v>0.853</v>
+        <v>0.839</v>
       </c>
       <c r="G10" t="n">
-        <v>0.264</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="11">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.025</v>
+        <v>0.001</v>
       </c>
       <c r="C11" t="n">
-        <v>1.627</v>
+        <v>1.642</v>
       </c>
       <c r="D11" t="n">
-        <v>0.615</v>
+        <v>0.63</v>
       </c>
       <c r="E11" t="n">
-        <v>0.784</v>
+        <v>0.794</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.679</v>
       </c>
       <c r="G11" t="n">
-        <v>0.209</v>
+        <v>0.261</v>
       </c>
     </row>
     <row r="12">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.169</v>
+        <v>-0.004</v>
       </c>
       <c r="C12" t="n">
-        <v>1.752</v>
+        <v>1.645</v>
       </c>
       <c r="D12" t="n">
-        <v>0.353</v>
+        <v>0.303</v>
       </c>
       <c r="E12" t="n">
-        <v>0.594</v>
+        <v>0.55</v>
       </c>
       <c r="F12" t="n">
-        <v>0.445</v>
+        <v>0.43</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.47</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="13">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.083</v>
+        <v>-0.07099999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>1.696</v>
+        <v>1.688</v>
       </c>
       <c r="D13" t="n">
-        <v>0.528</v>
+        <v>0.523</v>
       </c>
       <c r="E13" t="n">
-        <v>0.727</v>
+        <v>0.723</v>
       </c>
       <c r="F13" t="n">
-        <v>0.668</v>
+        <v>0.674</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.162</v>
+        <v>0.466</v>
       </c>
     </row>
     <row r="14">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.133</v>
+        <v>-0.063</v>
       </c>
       <c r="C14" t="n">
-        <v>1.728</v>
+        <v>1.683</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.532</v>
       </c>
       <c r="E14" t="n">
-        <v>0.752</v>
+        <v>0.729</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.534</v>
       </c>
       <c r="G14" t="n">
-        <v>0.047</v>
+        <v>0.437</v>
       </c>
     </row>
     <row r="15">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.052</v>
+        <v>0.006</v>
       </c>
       <c r="C15" t="n">
-        <v>1.676</v>
+        <v>1.639</v>
       </c>
       <c r="D15" t="n">
-        <v>0.414</v>
+        <v>0.391</v>
       </c>
       <c r="E15" t="n">
-        <v>0.643</v>
+        <v>0.625</v>
       </c>
       <c r="F15" t="n">
-        <v>0.511</v>
+        <v>0.508</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.24</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="16">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-1.281</v>
+        <v>-0.982</v>
       </c>
       <c r="C16" t="n">
-        <v>1.48</v>
+        <v>1.417</v>
       </c>
       <c r="D16" t="n">
-        <v>0.247</v>
+        <v>0.215</v>
       </c>
       <c r="E16" t="n">
-        <v>0.497</v>
+        <v>0.464</v>
       </c>
       <c r="F16" t="n">
-        <v>0.431</v>
+        <v>0.425</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.471</v>
+        <v>0.351</v>
       </c>
     </row>
     <row r="17">
@@ -847,19 +847,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-5.306</v>
+        <v>-2.041</v>
       </c>
       <c r="C17" t="n">
-        <v>1.287</v>
+        <v>1.138</v>
       </c>
       <c r="D17" t="n">
-        <v>0.48</v>
+        <v>0.231</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.481</v>
       </c>
       <c r="F17" t="n">
-        <v>0.603</v>
+        <v>0.394</v>
       </c>
       <c r="G17" t="n">
         <v>-1</v>
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-6.958</v>
+        <v>-7.694</v>
       </c>
       <c r="C18" t="n">
-        <v>1.362</v>
+        <v>1.395</v>
       </c>
       <c r="D18" t="n">
-        <v>0.159</v>
+        <v>0.174</v>
       </c>
       <c r="E18" t="n">
-        <v>0.399</v>
+        <v>0.417</v>
       </c>
       <c r="F18" t="n">
-        <v>0.387</v>
+        <v>0.391</v>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-4.989</v>
+        <v>-12.55</v>
       </c>
       <c r="C19" t="n">
-        <v>1.272</v>
+        <v>1.616</v>
       </c>
       <c r="D19" t="n">
-        <v>0.302</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.55</v>
+        <v>0.827</v>
       </c>
       <c r="F19" t="n">
-        <v>0.511</v>
+        <v>0.788</v>
       </c>
       <c r="G19" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20">
@@ -922,19 +922,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-36.83</v>
+        <v>-9.769</v>
       </c>
       <c r="C20" t="n">
-        <v>2.72</v>
+        <v>1.49</v>
       </c>
       <c r="D20" t="n">
-        <v>1.181</v>
+        <v>0.336</v>
       </c>
       <c r="E20" t="n">
-        <v>1.087</v>
+        <v>0.58</v>
       </c>
       <c r="F20" t="n">
-        <v>1.083</v>
+        <v>0.556</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-76.893</v>
+        <v>-64.40900000000001</v>
       </c>
       <c r="C21" t="n">
-        <v>4.541</v>
+        <v>3.973</v>
       </c>
       <c r="D21" t="n">
-        <v>2.105</v>
+        <v>1.768</v>
       </c>
       <c r="E21" t="n">
-        <v>1.451</v>
+        <v>1.33</v>
       </c>
       <c r="F21" t="n">
-        <v>1.423</v>
+        <v>1.321</v>
       </c>
       <c r="G21" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-24.725</v>
+        <v>-10.36</v>
       </c>
       <c r="C22" t="n">
-        <v>2.169</v>
+        <v>1.516</v>
       </c>
       <c r="D22" t="n">
-        <v>0.874</v>
+        <v>0.386</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9350000000000001</v>
+        <v>0.621</v>
       </c>
       <c r="F22" t="n">
-        <v>0.921</v>
+        <v>0.591</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23">
@@ -997,19 +997,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-9.326000000000001</v>
+        <v>-8.734999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>1.469</v>
+        <v>1.442</v>
       </c>
       <c r="D23" t="n">
-        <v>1.63</v>
+        <v>1.537</v>
       </c>
       <c r="E23" t="n">
-        <v>1.277</v>
+        <v>1.24</v>
       </c>
       <c r="F23" t="n">
-        <v>1.069</v>
+        <v>1.147</v>
       </c>
       <c r="G23" t="n">
         <v>-1</v>
@@ -1022,19 +1022,19 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-1.675</v>
+        <v>-0.2</v>
       </c>
       <c r="C24" t="n">
-        <v>1.122</v>
+        <v>1.055</v>
       </c>
       <c r="D24" t="n">
-        <v>1.753</v>
+        <v>0.786</v>
       </c>
       <c r="E24" t="n">
-        <v>1.324</v>
+        <v>0.887</v>
       </c>
       <c r="F24" t="n">
-        <v>0.919</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G24" t="n">
         <v>-1</v>
@@ -1047,19 +1047,19 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.497</v>
+        <v>-6.954</v>
       </c>
       <c r="C25" t="n">
-        <v>1.068</v>
+        <v>1.362</v>
       </c>
       <c r="D25" t="n">
-        <v>0.106</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="E25" t="n">
-        <v>0.326</v>
+        <v>0.752</v>
       </c>
       <c r="F25" t="n">
-        <v>0.324</v>
+        <v>0.718</v>
       </c>
       <c r="G25" t="n">
         <v>1</v>
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-124.058</v>
+        <v>-0.316</v>
       </c>
       <c r="C26" t="n">
-        <v>6.684</v>
+        <v>1.06</v>
       </c>
       <c r="D26" t="n">
-        <v>1.356</v>
+        <v>0.014</v>
       </c>
       <c r="E26" t="n">
-        <v>1.164</v>
+        <v>0.118</v>
       </c>
       <c r="F26" t="n">
-        <v>1.152</v>
+        <v>0.113</v>
       </c>
       <c r="G26" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-1.204</v>
+        <v>-0.574</v>
       </c>
       <c r="C27" t="n">
-        <v>1.1</v>
+        <v>1.072</v>
       </c>
       <c r="D27" t="n">
-        <v>2.788</v>
+        <v>1.991</v>
       </c>
       <c r="E27" t="n">
-        <v>1.67</v>
+        <v>1.411</v>
       </c>
       <c r="F27" t="n">
         <v>1.125</v>
       </c>
       <c r="G27" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-4.599</v>
+        <v>-2.348</v>
       </c>
       <c r="C28" t="n">
-        <v>1.254</v>
+        <v>1.152</v>
       </c>
       <c r="D28" t="n">
-        <v>0.863</v>
+        <v>0.516</v>
       </c>
       <c r="E28" t="n">
-        <v>0.929</v>
+        <v>0.718</v>
       </c>
       <c r="F28" t="n">
-        <v>0.837</v>
+        <v>0.625</v>
       </c>
       <c r="G28" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-9805.931</v>
+        <v>-6979.821</v>
       </c>
       <c r="C29" t="n">
-        <v>446.77</v>
+        <v>318.31</v>
       </c>
       <c r="D29" t="n">
-        <v>11.474</v>
+        <v>8.167</v>
       </c>
       <c r="E29" t="n">
-        <v>3.387</v>
+        <v>2.858</v>
       </c>
       <c r="F29" t="n">
-        <v>3.383</v>
+        <v>2.857</v>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.772</v>
+        <v>-0.049</v>
       </c>
       <c r="C30" t="n">
-        <v>1.081</v>
+        <v>1.048</v>
       </c>
       <c r="D30" t="n">
-        <v>0.135</v>
+        <v>0.08</v>
       </c>
       <c r="E30" t="n">
-        <v>0.367</v>
+        <v>0.283</v>
       </c>
       <c r="F30" t="n">
         <v>0.276</v>
       </c>
       <c r="G30" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-26.621</v>
+        <v>-27.687</v>
       </c>
       <c r="C31" t="n">
-        <v>2.255</v>
+        <v>2.304</v>
       </c>
       <c r="D31" t="n">
-        <v>2.456</v>
+        <v>2.551</v>
       </c>
       <c r="E31" t="n">
-        <v>1.567</v>
+        <v>1.597</v>
       </c>
       <c r="F31" t="n">
-        <v>1.567</v>
+        <v>1.564</v>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="32">
@@ -1222,19 +1222,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-25.402</v>
+        <v>-10.554</v>
       </c>
       <c r="C32" t="n">
-        <v>2.2</v>
+        <v>1.525</v>
       </c>
       <c r="D32" t="n">
-        <v>3.222</v>
+        <v>1.41</v>
       </c>
       <c r="E32" t="n">
-        <v>1.795</v>
+        <v>1.187</v>
       </c>
       <c r="F32" t="n">
-        <v>1.692</v>
+        <v>1.123</v>
       </c>
       <c r="G32" t="n">
         <v>-1</v>
@@ -1243,101 +1243,101 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Pre2020NNavg</t>
+          <t>TotalNNAvg</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.1279285714285714</v>
+        <v>-52.86607878151261</v>
       </c>
       <c r="C33" t="n">
-        <v>1.725142857142857</v>
+        <v>3.924334033613445</v>
       </c>
       <c r="D33" t="n">
-        <v>1.210857142857143</v>
+        <v>0.9206848739495799</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9613571428571431</v>
+        <v>0.8078455882352942</v>
       </c>
       <c r="F33" t="n">
-        <v>0.8039285714285712</v>
+        <v>0.6905388655462186</v>
       </c>
       <c r="G33" t="n">
-        <v>0.02521428571428571</v>
+        <v>0.08210084033613443</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>TransNNavg</t>
+          <t>Pre2020NNavg</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-1.281</v>
+        <v>-0.08057142857142856</v>
       </c>
       <c r="C34" t="n">
-        <v>1.48</v>
+        <v>1.694642857142857</v>
       </c>
       <c r="D34" t="n">
-        <v>0.247</v>
+        <v>1.192714285714286</v>
       </c>
       <c r="E34" t="n">
-        <v>0.497</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="F34" t="n">
-        <v>0.431</v>
+        <v>0.7814285714285715</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.471</v>
+        <v>-0.01092857142857145</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Post2020NNavg</t>
+          <t>TransNNavg</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-634.736625</v>
+        <v>-0.982</v>
       </c>
       <c r="C35" t="n">
-        <v>29.897125</v>
+        <v>1.417</v>
       </c>
       <c r="D35" t="n">
-        <v>1.93025</v>
+        <v>0.215</v>
       </c>
       <c r="E35" t="n">
-        <v>1.1825625</v>
+        <v>0.464</v>
       </c>
       <c r="F35" t="n">
-        <v>1.0795</v>
+        <v>0.425</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.125</v>
+        <v>0.351</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>TotalNNAvg</t>
+          <t>Post2020NNavg</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-75.12691386554623</v>
+        <v>-446.5038125</v>
       </c>
       <c r="C36" t="n">
-        <v>4.967392857142857</v>
+        <v>21.341125</v>
       </c>
       <c r="D36" t="n">
-        <v>1.012004201680673</v>
+        <v>1.32475</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8508056722689077</v>
+        <v>0.9566875</v>
       </c>
       <c r="F36" t="n">
-        <v>0.7266638655462183</v>
+        <v>0.8999374999999999</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.1384033613445378</v>
+        <v>-0.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>